<commit_message>
ongoing work, csv added, better views
</commit_message>
<xml_diff>
--- a/doc/paxlist/pax02.xlsx
+++ b/doc/paxlist/pax02.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="pax01.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:wis:Documents:Dev:PaxListConverter:doc:paxlist:pax01.txt" thousands=" ">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:wis:Documents:Dev:PaxListConverter:doc:paxlist:pax01.txt" thousands=" ">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -60,9 +60,6 @@
     <t>TypeOfID</t>
   </si>
   <si>
-    <t>serialnrID</t>
-  </si>
-  <si>
     <t>serialNrVisa</t>
   </si>
   <si>
@@ -99,12 +96,6 @@
     <t>Leuven</t>
   </si>
   <si>
-    <t>ExpDate_DD/MM/YY</t>
-  </si>
-  <si>
-    <t>DoB_/DD/MM/YY</t>
-  </si>
-  <si>
     <t>Harry</t>
   </si>
   <si>
@@ -118,6 +109,15 @@
   </si>
   <si>
     <t>London</t>
+  </si>
+  <si>
+    <t>ExpDate_Excel</t>
+  </si>
+  <si>
+    <t>DoB_Excel</t>
+  </si>
+  <si>
+    <t>serialNrID</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -528,33 +528,33 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
       <c r="F2">
         <v>123456789</v>
@@ -566,24 +566,24 @@
         <v>20879</v>
       </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>987654321</v>
@@ -595,24 +595,24 @@
         <v>34824</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
       </c>
       <c r="G4">
         <v>12345</v>
@@ -624,7 +624,7 @@
         <v>36526</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting with the Filter Factory, lots of progress done
</commit_message>
<xml_diff>
--- a/doc/paxlist/pax02.xlsx
+++ b/doc/paxlist/pax02.xlsx
@@ -114,10 +114,10 @@
     <t>ExpDate_Excel</t>
   </si>
   <si>
-    <t>DoB_Excel</t>
-  </si>
-  <si>
     <t>serialNrID</t>
+  </si>
+  <si>
+    <t>BirthDate_Excel</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -528,7 +528,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -537,7 +537,7 @@
         <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>

</xml_diff>